<commit_message>
Excel formatting changed, still need to fix % bug
</commit_message>
<xml_diff>
--- a/comparative_analysis.xlsx
+++ b/comparative_analysis.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,13 +28,23 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00000080"/>
+        <bgColor rgb="00000080"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,14 +65,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -428,50 +440,205 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="13" bestFit="1" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Debt ratio</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>EPS</t>
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Cash ratio</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Gross profit margin</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Return on equity</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Operating cash flow</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Days of payables outstanding</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Ebitgrowth</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Interest expense</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Current debt</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Cost of revenue</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>NVDA</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.2878684862318489</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4.13</v>
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>0.6085214721629413</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>0.25598438535759</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.2814736936292054</v>
+      </c>
+      <c r="E2" t="n">
+        <v>13956</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>91.86878186407959</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7622227014997984</v>
+      </c>
+      <c r="H2" t="n">
+        <v>143</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1502</v>
+      </c>
+      <c r="J2" t="n">
+        <v>73825</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>TSLA</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.03763754281133863</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3.1</v>
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>0.2100731576234192</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>0.1338628895907104</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1465364644795846</v>
+      </c>
+      <c r="E3" t="n">
+        <v>22897</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>73.90124784536735</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-0.5562100638977636</v>
+      </c>
+      <c r="H3" t="n">
+        <v>957</v>
+      </c>
+      <c r="I3" t="n">
+        <v>38778</v>
+      </c>
+      <c r="J3" t="n">
+        <v>150139</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>0.2594718477071418</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>0.1496928323326395</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.04976643078488507</v>
+      </c>
+      <c r="E4" t="n">
+        <v>12825</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>69.53894060135271</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.3540207679304516</v>
+      </c>
+      <c r="H4" t="n">
+        <v>9505</v>
+      </c>
+      <c r="I4" t="n">
+        <v>50164</v>
+      </c>
+      <c r="J4" t="n">
+        <v>144310</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>0.4337335684024101</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>0.1044072101070701</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.6048686189323729</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" s="4" t="n">
+        <v>208.6512383532004</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-0.9370994324123324</v>
+      </c>
+      <c r="H5" t="n">
+        <v>342.268</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5277.126</v>
+      </c>
+      <c r="J5" t="n">
+        <v>45907.719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fix + natural language SQL query file started
</commit_message>
<xml_diff>
--- a/comparative_analysis.xlsx
+++ b/comparative_analysis.xlsx
@@ -71,7 +71,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,192 +453,122 @@
     <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="13" bestFit="1" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Cash ratio</t>
+          <t>Long-term debt</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Gross profit margin</t>
+          <t>Gross profit</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Return on equity</t>
+          <t>Price to free cash flows ratio</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Operating cash flow</t>
+          <t>Price to book ratio</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Days of payables outstanding</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Ebitgrowth</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Interest expense</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>Current debt</t>
-        </is>
-      </c>
-      <c r="J1" s="2" t="inlineStr">
-        <is>
-          <t>Cost of revenue</t>
+          <t>Price to sales ratio</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>TSLA</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>0.6085214721629413</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>0.25598438535759</v>
+          <t>UAL</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>28283</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15082</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2814736936292054</v>
-      </c>
-      <c r="E2" t="n">
-        <v>13956</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>91.86878186407959</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.7622227014997984</v>
-      </c>
-      <c r="H2" t="n">
-        <v>143</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1502</v>
-      </c>
-      <c r="J2" t="n">
-        <v>73825</v>
+        <v>9.789629593023255</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>1.770253495142111</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.2715530664553442</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>GM</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>0.2100731576234192</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>0.1338628895907104</v>
+          <t>AAL</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>32389</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12439</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1465364644795846</v>
-      </c>
-      <c r="E3" t="n">
-        <v>22897</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>73.90124784536735</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-0.5562100638977636</v>
-      </c>
-      <c r="H3" t="n">
-        <v>957</v>
-      </c>
-      <c r="I3" t="n">
-        <v>38778</v>
-      </c>
-      <c r="J3" t="n">
-        <v>150139</v>
+        <v>-11.28565948158254</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>-1.426519813760993</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.1689242286251046</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>0.2594718477071418</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>0.1496928323326395</v>
+          <t>LUV</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>8046</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4503</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.04976643078488507</v>
-      </c>
-      <c r="E4" t="n">
-        <v>12825</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>69.53894060135271</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-0.3540207679304516</v>
-      </c>
-      <c r="H4" t="n">
-        <v>9505</v>
-      </c>
-      <c r="I4" t="n">
-        <v>50164</v>
-      </c>
-      <c r="J4" t="n">
-        <v>144310</v>
+        <v>-127.9891666666667</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>1.868280153457472</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8384273956496179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>NIO</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>0.4337335684024101</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>0.1044072101070701</v>
+          <t>SAVE</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3200.376</v>
+      </c>
+      <c r="C5" t="n">
+        <v>799.317</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.6048686189323729</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" s="4" t="n">
-        <v>208.6512383532004</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-0.9370994324123324</v>
-      </c>
-      <c r="H5" t="n">
-        <v>342.268</v>
-      </c>
-      <c r="I5" t="n">
-        <v>5277.126</v>
-      </c>
-      <c r="J5" t="n">
-        <v>45907.719</v>
+        <v>-5.996743227559657</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>1.347926148998728</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.4179721086163079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new page after selecting companies. New page allows user to select metrics for selected companies
</commit_message>
<xml_diff>
--- a/comparative_analysis.xlsx
+++ b/comparative_analysis.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,123 +452,67 @@
     <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Long-term debt</t>
+          <t>Debt equity ratio</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Gross profit</t>
+          <t>Interest coverage</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Price to free cash flows ratio</t>
+          <t>Revenue growth</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Price to book ratio</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Price to sales ratio</t>
+          <t>Retained earnings</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>UAL</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>28283</v>
-      </c>
-      <c r="C2" t="n">
-        <v>15082</v>
+        <v>1.787532584558942</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>29.06203915586067</v>
       </c>
       <c r="D2" t="n">
-        <v>9.789629593023255</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>1.770253495142111</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.2715530664553442</v>
+        <v>-0.02041077580526742</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-214000000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>AAL</t>
+          <t>SONY</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32389</v>
-      </c>
-      <c r="C3" t="n">
-        <v>12439</v>
+        <v>0.5620591368200297</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>20.49508914182966</v>
       </c>
       <c r="D3" t="n">
-        <v>-11.28565948158254</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>-1.426519813760993</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.1689242286251046</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>LUV</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>8046</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4503</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-127.9891666666667</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>1.868280153457472</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.8384273956496179</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>SAVE</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3200.376</v>
-      </c>
-      <c r="C5" t="n">
-        <v>799.317</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-5.996743227559657</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>1.347926148998728</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.4179721086163079</v>
+        <v>0.014244529073212</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4614637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Statis metricsdb added locally
</commit_message>
<xml_diff>
--- a/comparative_analysis.xlsx
+++ b/comparative_analysis.xlsx
@@ -65,7 +65,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -74,7 +74,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -440,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,67 +451,311 @@
     <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="13" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="13" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="13" bestFit="1" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Debt equity ratio</t>
+          <t>ticker</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Interest coverage</t>
+          <t>Debt growth</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Revenue growth</t>
+          <t>Net income available to common shareholders</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Retained earnings</t>
+          <t>Other working capital</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Net income per EBT</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Dividend yield</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Operating cash flow sales ratio</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Current ratio</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Total liabilities</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Debt repayment</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Net cash used provided by (used for) financing activities</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>AAPL</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1.787532584558942</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>29.06203915586067</v>
+      <c r="C2" t="n">
+        <v>-0.05621795375732642</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.02041077580526742</v>
+        <v>94760</v>
       </c>
       <c r="E2" t="n">
-        <v>-214000000</v>
+        <v>100987</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8528082577196314</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.005573960673721321</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.2884094081427658</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9880116717592975</v>
+      </c>
+      <c r="J2" t="n">
+        <v>290437</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-13944000000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-112129000000</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>SONY</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.5620591368200297</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>20.49508914182966</v>
+      <c r="A3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.006</v>
       </c>
       <c r="D3" t="n">
-        <v>0.014244529073212</v>
+        <v>10326</v>
       </c>
       <c r="E3" t="n">
-        <v>4614637</v>
+        <v>10323</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.044726142071275</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0008351537797192516</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.2091273077778601</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3.515617857687033</v>
+      </c>
+      <c r="J3" t="n">
+        <v>19081</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1250000000</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-10888000000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.04906924009914043</v>
+      </c>
+      <c r="D4" t="n">
+        <v>20079</v>
+      </c>
+      <c r="E4" t="n">
+        <v>16921</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.4583263175618791</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.09096020685509054</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9446435811136924</v>
+      </c>
+      <c r="J4" t="n">
+        <v>316632</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-45272000000</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-9047000000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0108339632149156</v>
+      </c>
+      <c r="D5" t="n">
+        <v>66732</v>
+      </c>
+      <c r="E5" t="n">
+        <v>77618</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8407918349035441</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.3234913518788273</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2.377994227994228</v>
+      </c>
+      <c r="J5" t="n">
+        <v>109120</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-18339000000</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-70414000000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.04207412477997262</v>
+      </c>
+      <c r="D6" t="n">
+        <v>77096</v>
+      </c>
+      <c r="E6" t="n">
+        <v>63226</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.8102137474667174</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.007777998514954823</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.4132883467427978</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.76916725076573</v>
+      </c>
+      <c r="J6" t="n">
+        <v>205753</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-3250000000</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-18291000000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0108339632149156</v>
+      </c>
+      <c r="D7" t="n">
+        <v>66732</v>
+      </c>
+      <c r="E7" t="n">
+        <v>77618</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8407918349035441</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.3234913518788273</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2.377994227994228</v>
+      </c>
+      <c r="J7" t="n">
+        <v>109120</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-18339000000</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-70414000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gitignore for api key
</commit_message>
<xml_diff>
--- a/comparative_analysis.xlsx
+++ b/comparative_analysis.xlsx
@@ -42,8 +42,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00000080"/>
-        <bgColor rgb="00000080"/>
+        <fgColor rgb="001F497D"/>
+        <bgColor rgb="001F497D"/>
       </patternFill>
     </fill>
   </fills>
@@ -65,12 +65,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -439,24 +436,35 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="13" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="13" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="6" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="9" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="7" max="7"/>
+    <col width="9" customWidth="1" min="8" max="8"/>
+    <col width="7" customWidth="1" min="9" max="9"/>
+    <col width="7" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="9" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="11" customWidth="1" min="15" max="15"/>
+    <col width="22" customWidth="1" min="16" max="16"/>
+    <col width="21" customWidth="1" min="17" max="17"/>
+    <col width="9" customWidth="1" min="18" max="18"/>
+    <col width="6" customWidth="1" min="19" max="19"/>
+    <col width="6" customWidth="1" min="20" max="20"/>
+    <col width="6" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,115 +476,426 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
+          <t>Total revenue_1</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Current debt_1</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Enterprise value multiple_1</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Free cash flow_1</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Operating profit margin_1</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Gross profit margin_1</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Gross profit_1</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>PE ratio_1</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>PEG ratio_1</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
           <t>EBITDA_1</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Total operating expenses_1</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Current debt_1</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Total revenue_2</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>Current debt_2</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>Enterprise value multiple_2</t>
+        </is>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>Free cash flow_2</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="inlineStr">
+        <is>
+          <t>Operating profit margin_2</t>
+        </is>
+      </c>
+      <c r="R1" s="2" t="inlineStr">
+        <is>
+          <t>Gross profit margin_2</t>
+        </is>
+      </c>
+      <c r="S1" s="2" t="inlineStr">
+        <is>
+          <t>Gross profit_2</t>
+        </is>
+      </c>
+      <c r="T1" s="2" t="inlineStr">
+        <is>
+          <t>PE ratio_2</t>
+        </is>
+      </c>
+      <c r="U1" s="2" t="inlineStr">
+        <is>
+          <t>PEG ratio_2</t>
+        </is>
+      </c>
+      <c r="V1" s="2" t="inlineStr">
         <is>
           <t>EBITDA_2</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Total operating expenses_2</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Current debt_2</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>EBITDA_3</t>
-        </is>
-      </c>
-      <c r="J1" s="2" t="inlineStr">
-        <is>
-          <t>Total operating expenses_3</t>
-        </is>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>Current debt_3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>TSLA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>125820.002</v>
+        <v>24578</v>
       </c>
       <c r="D2" t="n">
-        <v>38668</v>
+        <v>1785</v>
       </c>
       <c r="E2" t="n">
-        <v>13769</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
+        <v>38.39821634371115</v>
+      </c>
+      <c r="F2" t="n">
+        <v>968</v>
+      </c>
       <c r="G2" t="n">
-        <v>43887</v>
+        <v>-0.01808248235845151</v>
       </c>
       <c r="H2" t="n">
-        <v>15613</v>
-      </c>
-      <c r="I2" t="inlineStr"/>
+        <v>0.1883402695497768</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4069</v>
+      </c>
       <c r="J2" t="n">
-        <v>51345</v>
+        <v>75.83</v>
       </c>
       <c r="K2" t="n">
-        <v>21110</v>
-      </c>
+        <v>1.281</v>
+      </c>
+      <c r="L2" t="n">
+        <v>15152</v>
+      </c>
+      <c r="M2" t="n">
+        <v>31536</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2132</v>
+      </c>
+      <c r="O2" t="n">
+        <v>35.02638398622471</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2701</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.006876068028318008</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.1655545609895028</v>
+      </c>
+      <c r="S2" t="n">
+        <v>6630</v>
+      </c>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>F</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>108530.999</v>
+        <v>155900</v>
       </c>
       <c r="D3" t="n">
-        <v>43978</v>
+        <v>53946</v>
       </c>
       <c r="E3" t="n">
-        <v>3749</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
+        <v>7.185627584117975</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10007</v>
+      </c>
       <c r="G3" t="n">
-        <v>45940</v>
+        <v>0.01668350609337774</v>
       </c>
       <c r="H3" t="n">
-        <v>8072</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
+        <v>0.1501141338921528</v>
+      </c>
+      <c r="I3" t="n">
+        <v>21207</v>
+      </c>
       <c r="J3" t="n">
-        <v>52237</v>
+        <v>6.71</v>
       </c>
       <c r="K3" t="n">
-        <v>2749</v>
-      </c>
+        <v>0.383</v>
+      </c>
+      <c r="L3" t="n">
+        <v>16908</v>
+      </c>
+      <c r="M3" t="n">
+        <v>127144</v>
+      </c>
+      <c r="N3" t="n">
+        <v>51343</v>
+      </c>
+      <c r="O3" t="n">
+        <v>9.635521277759544</v>
+      </c>
+      <c r="P3" t="n">
+        <v>18527</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.0628094932649134</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.1360295060936498</v>
+      </c>
+      <c r="S3" t="n">
+        <v>14392</v>
+      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>137237</v>
+      </c>
+      <c r="D4" t="n">
+        <v>37400</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.740609014995846</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-8975</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.03022801923168468</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.09585240294051643</v>
+      </c>
+      <c r="I4" t="n">
+        <v>13972</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3.937</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1.073</v>
+      </c>
+      <c r="L4" t="n">
+        <v>16681</v>
+      </c>
+      <c r="M4" t="n">
+        <v>122485</v>
+      </c>
+      <c r="N4" t="n">
+        <v>36913</v>
+      </c>
+      <c r="O4" t="n">
+        <v>6.105542621776504</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-3863</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.05988181029897185</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.1018092788387971</v>
+      </c>
+      <c r="S4" t="n">
+        <v>13672</v>
+      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>RIVN</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>-183.4747792207792</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-552</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>-5087000064</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>28</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-71.38510703363914</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1762</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LCID</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>-339.589</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-56.19477124183007</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.1446623093681917</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>-2866640896</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3.976</v>
+      </c>
+      <c r="N6" t="n">
+        <v>15.281</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.6188304231982364</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1029.778</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-150.7110160965795</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.2278672032193159</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.906</v>
+      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed years functionality. Now picking up the correct data from openbb API. Still need to add support for missing data for metrics
</commit_message>
<xml_diff>
--- a/comparative_analysis.xlsx
+++ b/comparative_analysis.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,6 @@
     <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
     <col width="13" bestFit="1" customWidth="1" min="8" max="8"/>
     <col width="13" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="13" bestFit="1" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,47 +467,42 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>EBITDA_1</t>
+          <t>Total revenue_TTM</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Total operating expenses_1</t>
+          <t>Free cash flow_TTM</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Current debt_1</t>
+          <t>Total revenue_2022</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>EBITDA_2</t>
+          <t>Free cash flow_2022</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>Total operating expenses_2</t>
+          <t>Total revenue_2021</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Current debt_2</t>
+          <t>Free cash flow_2021</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>EBITDA_3</t>
+          <t>Total revenue_2020</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>Total operating expenses_3</t>
-        </is>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>Current debt_3</t>
+          <t>Free cash flow_2020</t>
         </is>
       </c>
     </row>
@@ -522,60 +516,28 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>125820.002</v>
+        <v>383933000000</v>
       </c>
       <c r="D2" t="n">
-        <v>38668</v>
+        <v>100987000000</v>
       </c>
       <c r="E2" t="n">
-        <v>13769</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
+        <v>394328000000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>111443000000</v>
+      </c>
       <c r="G2" t="n">
-        <v>43887</v>
+        <v>365817000000</v>
       </c>
       <c r="H2" t="n">
-        <v>15613</v>
-      </c>
-      <c r="I2" t="inlineStr"/>
+        <v>92953000000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>274515000000</v>
+      </c>
       <c r="J2" t="n">
-        <v>51345</v>
-      </c>
-      <c r="K2" t="n">
-        <v>21110</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MSFT</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>108530.999</v>
-      </c>
-      <c r="D3" t="n">
-        <v>43978</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3749</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>45940</v>
-      </c>
-      <c r="H3" t="n">
-        <v>8072</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>52237</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2749</v>
+        <v>73365000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>